<commit_message>
Withdraw the key from CJN
</commit_message>
<xml_diff>
--- a/信北A321钥匙记录表-王超.xlsx
+++ b/信北A321钥匙记录表-王超.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>郑海永</t>
   </si>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>（目前共6把，使用6把，闲置0把）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>常琳</t>
     <rPh sb="0" eb="1">
       <t>chang lin</t>
@@ -86,6 +82,17 @@
     <rPh sb="0" eb="1">
       <t>cui jin n</t>
     </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>20170208收回</t>
+    <rPh sb="8" eb="9">
+      <t>shou hui</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>（目前共6把，使用5把，闲置1把）</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -421,7 +428,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -440,7 +447,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -482,7 +489,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -490,6 +497,9 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Withdraw the key from WC and CL
</commit_message>
<xml_diff>
--- a/信北A321钥匙记录表-王超.xlsx
+++ b/信北A321钥匙记录表-王超.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>郑海永</t>
   </si>
@@ -92,7 +92,21 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>（目前共6把，使用5把，闲置1把）</t>
+    <t>20170214收回</t>
+    <rPh sb="8" eb="9">
+      <t>shou hui</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>20170209收回</t>
+    <rPh sb="8" eb="9">
+      <t>shou hui</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>（目前共6把，使用3把，闲置3把）</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -428,7 +442,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -447,7 +461,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -475,6 +489,9 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
@@ -490,6 +507,9 @@
       </c>
       <c r="B6" t="s">
         <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Withdraw the key from ZZQ
</commit_message>
<xml_diff>
--- a/信北A321钥匙记录表-王超.xlsx
+++ b/信北A321钥匙记录表-王超.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>郑海永</t>
   </si>
@@ -106,7 +106,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>（目前共6把，使用3把，闲置3把）</t>
+    <t>（目前共6把，使用2把，闲置4把）</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -442,7 +442,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -499,6 +499,9 @@
       </c>
       <c r="B5" t="s">
         <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Grant one key to CuiJinna
</commit_message>
<xml_diff>
--- a/信北A321钥匙记录表-王超.xlsx
+++ b/信北A321钥匙记录表-王超.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>郑海永</t>
   </si>
@@ -106,7 +106,14 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>（目前共6把，使用2把，闲置4把）</t>
+    <t>（目前共6把，使用3把，闲置3把）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>20170331给予</t>
+    <rPh sb="8" eb="9">
+      <t>gei yu</t>
+    </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -442,7 +449,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -524,6 +531,9 @@
       </c>
       <c r="C7" t="s">
         <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>